<commit_message>
get units from JRC_EU_TIMES model update
</commit_message>
<xml_diff>
--- a/Inputs/TIMES_EV_Capacities.xlsx
+++ b/Inputs/TIMES_EV_Capacities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17058D2-F7C3-4EC9-983F-D4F0C118C3C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E400A7DB-AB6B-4150-860C-0F9C9893D1A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2BF38A4-E098-4FE1-822E-30B11FE498F9}"/>
+    <workbookView xWindow="5655" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{C2BF38A4-E098-4FE1-822E-30B11FE498F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>LV</t>
   </si>
   <si>
-    <t>Mt</t>
-  </si>
-  <si>
     <t>NL</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>MT</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +753,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1">
         <v>1.4379999999999999</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>119.73399999999999</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>32.164000000000001</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
         <v>100.548</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
         <v>66.706000000000003</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>35.165999999999997</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>59.588000000000001</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
         <v>18.103999999999999</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>11.965999999999999</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
         <v>285.23599999999999</v>

</xml_diff>